<commit_message>
Add AFIO presentation slides for CppCon and ACCU.
</commit_message>
<xml_diff>
--- a/graphs/benchmark_locking 2x i5 M540 @ 2.53Ghz Win10 4.125Gb bandwidth.xlsx
+++ b/graphs/benchmark_locking 2x i5 M540 @ 2.53Ghz Win10 4.125Gb bandwidth.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="32">
   <si>
     <t>lock_files</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>FAT32</t>
+  </si>
+  <si>
+    <t>exFAT</t>
   </si>
 </sst>
 </file>
@@ -5256,8 +5259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH113" workbookViewId="0">
-      <selection activeCell="BA149" sqref="BA149"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AI60" sqref="AI60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5324,6 +5327,17 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
+      <c r="AE4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
     </row>
     <row r="5" spans="1:39">
       <c r="A5" t="s">
@@ -11278,13 +11292,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="U4:AC4"/>
+    <mergeCell ref="AE4:AM4"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:I25">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -11292,6 +11307,138 @@
         <color rgb="FF00FF00"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:I36">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00FF00"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:I14">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00FF00"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:I36">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:I69">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40:I47">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B51:I58">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:I69">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7:S14">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18:S25">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11303,15 +11450,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:I36">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="L29:S36">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11323,59 +11462,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:I14">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:I36">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40:I69">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40:I47">
+  <conditionalFormatting sqref="L40:S47">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11387,7 +11474,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51:I58">
+  <conditionalFormatting sqref="L51:S58">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11399,7 +11486,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:I69">
+  <conditionalFormatting sqref="L62:S69">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11411,7 +11498,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:S14">
+  <conditionalFormatting sqref="V62:AC69">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11423,7 +11510,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18:S25">
+  <conditionalFormatting sqref="V51:AC58">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11435,7 +11522,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L29:S36">
+  <conditionalFormatting sqref="V40:AC47">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11447,7 +11534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:S47">
+  <conditionalFormatting sqref="V29:AC36">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11459,7 +11546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L51:S58">
+  <conditionalFormatting sqref="V18:AC25">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11471,7 +11558,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62:S69">
+  <conditionalFormatting sqref="V7:AC14">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11483,7 +11570,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V62:AC69">
+  <conditionalFormatting sqref="AF7:AM14">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11495,7 +11582,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V51:AC58">
+  <conditionalFormatting sqref="AF18:AM25">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11507,7 +11594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V40:AC47">
+  <conditionalFormatting sqref="AF29:AM36">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11519,7 +11606,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V29:AC36">
+  <conditionalFormatting sqref="AF40:AM47">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11531,7 +11618,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V18:AC25">
+  <conditionalFormatting sqref="AF51:AM58">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11543,7 +11630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V7:AC14">
+  <conditionalFormatting sqref="AF62:AM69">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11556,7 +11643,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor fixes from writing CppCon slides
</commit_message>
<xml_diff>
--- a/graphs/benchmark_locking 2x i5 M540 @ 2.53Ghz Win10 4.125Gb bandwidth.xlsx
+++ b/graphs/benchmark_locking 2x i5 M540 @ 2.53Ghz Win10 4.125Gb bandwidth.xlsx
@@ -379,11 +379,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="48079616"/>
-        <c:axId val="48081920"/>
+        <c:axId val="105871616"/>
+        <c:axId val="105886464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48079616"/>
+        <c:axId val="105871616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,14 +407,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48081920"/>
+        <c:crossAx val="105886464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48081920"/>
+        <c:axId val="105886464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48079616"/>
+        <c:crossAx val="105871616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -463,7 +463,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -497,6 +497,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -631,12 +632,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>memory map</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7489908</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6526982</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5453116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4565350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3886815</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3296295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2907728</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2301558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51135616"/>
-        <c:axId val="51137536"/>
+        <c:axId val="134691456"/>
+        <c:axId val="134701824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51135616"/>
+        <c:axId val="134691456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,16 +701,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51137536"/>
+        <c:crossAx val="134701824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51137536"/>
+        <c:axId val="134701824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -690,16 +735,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51135616"/>
+        <c:crossAx val="134691456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -715,7 +762,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -749,6 +796,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -884,11 +932,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51176192"/>
-        <c:axId val="51178112"/>
+        <c:axId val="134732032"/>
+        <c:axId val="134734208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51176192"/>
+        <c:axId val="134732032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,16 +957,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51178112"/>
+        <c:crossAx val="134734208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51178112"/>
+        <c:axId val="134734208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -942,16 +991,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51176192"/>
+        <c:crossAx val="134732032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -967,7 +1018,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1001,6 +1052,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1136,11 +1188,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51216768"/>
-        <c:axId val="51218688"/>
+        <c:axId val="134780800"/>
+        <c:axId val="134787072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51216768"/>
+        <c:axId val="134780800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,16 +1213,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51218688"/>
+        <c:crossAx val="134787072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51218688"/>
+        <c:axId val="134787072"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1194,16 +1247,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51216768"/>
+        <c:crossAx val="134780800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1219,7 +1274,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1364,11 +1419,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51325952"/>
-        <c:axId val="51336320"/>
+        <c:axId val="134886144"/>
+        <c:axId val="134888064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51325952"/>
+        <c:axId val="134886144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,14 +1447,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51336320"/>
+        <c:crossAx val="134888064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51336320"/>
+        <c:axId val="134888064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1485,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51325952"/>
+        <c:crossAx val="134886144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1453,7 +1508,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1598,11 +1653,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51357568"/>
-        <c:axId val="51376128"/>
+        <c:axId val="134921600"/>
+        <c:axId val="134817280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51357568"/>
+        <c:axId val="134921600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,14 +1681,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51376128"/>
+        <c:crossAx val="134817280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51376128"/>
+        <c:axId val="134817280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +1719,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51357568"/>
+        <c:crossAx val="134921600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1687,7 +1742,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1721,6 +1776,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1856,11 +1912,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51291648"/>
-        <c:axId val="51293568"/>
+        <c:axId val="134839296"/>
+        <c:axId val="134845568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51291648"/>
+        <c:axId val="134839296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,16 +1937,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51293568"/>
+        <c:crossAx val="134845568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51293568"/>
+        <c:axId val="134845568"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1914,16 +1971,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51291648"/>
+        <c:crossAx val="134839296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1939,7 +1998,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1973,6 +2032,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2108,11 +2168,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51381376"/>
-        <c:axId val="51383296"/>
+        <c:axId val="134937216"/>
+        <c:axId val="134951680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51381376"/>
+        <c:axId val="134937216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,16 +2193,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51383296"/>
+        <c:crossAx val="134951680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51383296"/>
+        <c:axId val="134951680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2166,16 +2227,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51381376"/>
+        <c:crossAx val="134937216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2191,7 +2254,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2404,11 +2467,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="47543808"/>
-        <c:axId val="47545728"/>
+        <c:axId val="105790464"/>
+        <c:axId val="105809024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47543808"/>
+        <c:axId val="105790464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,14 +2495,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47545728"/>
+        <c:crossAx val="105809024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47545728"/>
+        <c:axId val="105809024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2465,7 +2528,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47543808"/>
+        <c:crossAx val="105790464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2488,7 +2551,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2522,6 +2585,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2700,11 +2764,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50878336"/>
-        <c:axId val="50888704"/>
+        <c:axId val="106237312"/>
+        <c:axId val="106243584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50878336"/>
+        <c:axId val="106237312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2725,16 +2789,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50888704"/>
+        <c:crossAx val="106243584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50888704"/>
+        <c:axId val="106243584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2756,16 +2821,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50878336"/>
+        <c:crossAx val="106237312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2781,7 +2848,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2950,12 +3017,55 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>memory map</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$87:$I$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>23160368</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19281835</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15828498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13340026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11223470</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9553637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8334436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6749962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50918912"/>
-        <c:axId val="50920832"/>
+        <c:axId val="106298368"/>
+        <c:axId val="134419584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50918912"/>
+        <c:axId val="106298368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2979,14 +3089,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50920832"/>
+        <c:crossAx val="134419584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50920832"/>
+        <c:axId val="134419584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3014,7 +3124,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50918912"/>
+        <c:crossAx val="106298368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3037,7 +3147,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3207,11 +3317,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96756864"/>
-        <c:axId val="96758784"/>
+        <c:axId val="134445696"/>
+        <c:axId val="134456064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96756864"/>
+        <c:axId val="134445696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3235,14 +3345,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96758784"/>
+        <c:crossAx val="134456064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96758784"/>
+        <c:axId val="134456064"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3270,7 +3380,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96756864"/>
+        <c:crossAx val="134445696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3293,7 +3403,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3327,6 +3437,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3462,11 +3573,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50942720"/>
-        <c:axId val="50944640"/>
+        <c:axId val="134502656"/>
+        <c:axId val="134525312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50942720"/>
+        <c:axId val="134502656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3487,16 +3598,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50944640"/>
+        <c:crossAx val="134525312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50944640"/>
+        <c:axId val="134525312"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3520,16 +3632,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50942720"/>
+        <c:crossAx val="134502656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3545,7 +3659,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3586,6 +3700,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3764,11 +3879,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50979968"/>
-        <c:axId val="50981888"/>
+        <c:axId val="134544000"/>
+        <c:axId val="134550272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50979968"/>
+        <c:axId val="134544000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,16 +3904,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50981888"/>
+        <c:crossAx val="134550272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50981888"/>
+        <c:axId val="134550272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3820,16 +3936,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50979968"/>
+        <c:crossAx val="134544000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3845,7 +3963,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3887,6 +4005,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4065,11 +4184,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51029504"/>
-        <c:axId val="51031424"/>
+        <c:axId val="134597632"/>
+        <c:axId val="134608000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51029504"/>
+        <c:axId val="134597632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4090,16 +4209,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51031424"/>
+        <c:crossAx val="134608000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51031424"/>
+        <c:axId val="134608000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4121,16 +4241,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51029504"/>
+        <c:crossAx val="134597632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4146,7 +4268,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4188,6 +4310,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4366,11 +4489,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51090944"/>
-        <c:axId val="51092864"/>
+        <c:axId val="134638592"/>
+        <c:axId val="134648960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51090944"/>
+        <c:axId val="134638592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4391,16 +4514,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51092864"/>
+        <c:crossAx val="134648960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51092864"/>
+        <c:axId val="134648960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4422,16 +4546,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51090944"/>
+        <c:crossAx val="134638592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4447,7 +4573,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4817,16 +4943,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>91050</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>11925</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>591113</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>178613</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4847,15 +4973,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>91050</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>591113</xdr:colOff>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>135750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5225,8 +5351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L93" sqref="L93"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AN95" sqref="AN95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11791,7 +11917,47 @@
     <mergeCell ref="AE4:AM4"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:I25">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37:I47">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:I14">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -11810,8 +11976,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37:I47">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="B7:I28 B37:I47">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -11830,48 +11996,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:I14">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:I28 B37:I47">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="B51:I80">
     <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00FF00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51:I80">
-    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -11883,6 +12009,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:I58">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:I69">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B73:I80">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11894,7 +12044,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:I69">
+  <conditionalFormatting sqref="L7:S14">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11906,7 +12056,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:I80">
+  <conditionalFormatting sqref="L18:S25">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11918,7 +12068,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:S14">
+  <conditionalFormatting sqref="L29:S47">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11930,7 +12080,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18:S25">
+  <conditionalFormatting sqref="L51:S58">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11942,7 +12092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L29:S47">
+  <conditionalFormatting sqref="L62:S69">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11954,7 +12104,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L51:S58">
+  <conditionalFormatting sqref="L73:S80">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11966,7 +12116,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62:S69">
+  <conditionalFormatting sqref="V73:AC80">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11978,7 +12128,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L73:S80">
+  <conditionalFormatting sqref="V62:AC69">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11990,7 +12140,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V73:AC80">
+  <conditionalFormatting sqref="V51:AC58">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12002,7 +12152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V62:AC69">
+  <conditionalFormatting sqref="V29:AC47">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12014,7 +12164,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V51:AC58">
+  <conditionalFormatting sqref="V18:AC25">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12026,7 +12176,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V29:AC47">
+  <conditionalFormatting sqref="V7:AC14">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12038,7 +12188,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V18:AC25">
+  <conditionalFormatting sqref="AF7:AM14">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12050,7 +12200,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V7:AC14">
+  <conditionalFormatting sqref="AF18:AM25">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12062,7 +12212,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF7:AM14">
+  <conditionalFormatting sqref="AF29:AM47">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12074,7 +12224,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF18:AM25">
+  <conditionalFormatting sqref="AF51:AM58">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12086,7 +12236,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF29:AM47">
+  <conditionalFormatting sqref="AF62:AM69">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12098,7 +12248,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF51:AM58">
+  <conditionalFormatting sqref="AF73:AM80">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12110,8 +12260,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF62:AM69">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="B29:I36">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -12122,8 +12272,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF73:AM80">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="B84:I91">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -12131,30 +12281,6 @@
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29:I36">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B84:I91">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed up the boost-lite C++ Modules build support which had become stale, and Gaby wanted a repro for the ICE we see when turning on C++ Modules.
</commit_message>
<xml_diff>
--- a/graphs/benchmark_locking 2x i5 M540 @ 2.53Ghz Win10 4.125Gb bandwidth.xlsx
+++ b/graphs/benchmark_locking 2x i5 M540 @ 2.53Ghz Win10 4.125Gb bandwidth.xlsx
@@ -379,11 +379,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105871616"/>
-        <c:axId val="105886464"/>
+        <c:axId val="112253568"/>
+        <c:axId val="113452160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105871616"/>
+        <c:axId val="112253568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,14 +407,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105886464"/>
+        <c:crossAx val="113452160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105886464"/>
+        <c:axId val="113452160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105871616"/>
+        <c:crossAx val="112253568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -463,7 +463,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -676,11 +676,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134691456"/>
-        <c:axId val="134701824"/>
+        <c:axId val="141402880"/>
+        <c:axId val="141404800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134691456"/>
+        <c:axId val="141402880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,14 +704,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134701824"/>
+        <c:crossAx val="141404800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134701824"/>
+        <c:axId val="141404800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -739,7 +739,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134691456"/>
+        <c:crossAx val="141402880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -762,7 +762,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -796,7 +796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -932,11 +931,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134732032"/>
-        <c:axId val="134734208"/>
+        <c:axId val="141508992"/>
+        <c:axId val="141510912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134732032"/>
+        <c:axId val="141508992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,17 +956,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134734208"/>
+        <c:crossAx val="141510912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134734208"/>
+        <c:axId val="141510912"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -991,18 +989,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134732032"/>
+        <c:crossAx val="141508992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1018,7 +1014,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1052,7 +1048,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1188,11 +1183,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134780800"/>
-        <c:axId val="134787072"/>
+        <c:axId val="141553664"/>
+        <c:axId val="141555584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134780800"/>
+        <c:axId val="141553664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,17 +1208,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134787072"/>
+        <c:crossAx val="141555584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134787072"/>
+        <c:axId val="141555584"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1247,18 +1241,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134780800"/>
+        <c:crossAx val="141553664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1274,7 +1266,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1419,11 +1411,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134886144"/>
-        <c:axId val="134888064"/>
+        <c:axId val="141482624"/>
+        <c:axId val="141484800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134886144"/>
+        <c:axId val="141482624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,14 +1439,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134888064"/>
+        <c:crossAx val="141484800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134888064"/>
+        <c:axId val="141484800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1477,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134886144"/>
+        <c:crossAx val="141482624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1508,7 +1500,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1546,7 +1538,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1653,11 +1644,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134921600"/>
-        <c:axId val="134817280"/>
+        <c:axId val="141575680"/>
+        <c:axId val="141577600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134921600"/>
+        <c:axId val="141575680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1678,17 +1669,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134817280"/>
+        <c:crossAx val="141577600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134817280"/>
+        <c:axId val="141577600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,18 +1705,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134921600"/>
+        <c:crossAx val="141575680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1742,7 +1730,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1912,11 +1900,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134839296"/>
-        <c:axId val="134845568"/>
+        <c:axId val="141620352"/>
+        <c:axId val="141622272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134839296"/>
+        <c:axId val="141620352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,14 +1928,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134845568"/>
+        <c:crossAx val="141622272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134845568"/>
+        <c:axId val="141622272"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1975,7 +1963,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134839296"/>
+        <c:crossAx val="141620352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1998,7 +1986,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2032,7 +2020,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2168,11 +2155,311 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134937216"/>
-        <c:axId val="134951680"/>
+        <c:axId val="141665024"/>
+        <c:axId val="141666944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134937216"/>
+        <c:axId val="141665024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Entities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141666944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141666944"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Max ops/sec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141665024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Scaling of four concurrent users of the lock algorithms to entities on NTFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lock files</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$54:$I$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3742</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1884</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>906</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>746</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>440</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>byte ranges</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$65:$I$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1077461</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>535494</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>348619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>245531</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>197498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155970</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138553</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>118115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>atomic append</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$76:$I$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>86871</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87444</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87234</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89427</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85681</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>memory map</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$87:$I$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>23160368</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19281835</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15828498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13340026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11223470</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9553637</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8334436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6749962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="141709696"/>
+        <c:axId val="141711616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="141709696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,14 +2483,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134951680"/>
+        <c:crossAx val="141711616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134951680"/>
+        <c:axId val="141711616"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2231,7 +2518,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134937216"/>
+        <c:crossAx val="141709696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2247,14 +2534,318 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1600"/>
+        <a:defRPr sz="4000"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Scaling of two contended users of the lock algorithms to entities on NTFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lock files</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1058</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>byte ranges</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$19:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>395879</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>142159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120077</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76342</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45294</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>atomic append</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$30:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>83489</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79872</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70425</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76958</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77422</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81651</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>memory map</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="101600"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$41:$I$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7489908</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6526982</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5453116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4565350</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3886815</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3296295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2907728</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2301558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="49473408"/>
+        <c:axId val="71761920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="49473408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Entities</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71761920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71761920"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="100000000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Max ops/sec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49473408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="4000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2467,11 +3058,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105790464"/>
-        <c:axId val="105809024"/>
+        <c:axId val="113474944"/>
+        <c:axId val="113489408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105790464"/>
+        <c:axId val="113474944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,14 +3086,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105809024"/>
+        <c:crossAx val="113489408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105809024"/>
+        <c:axId val="113489408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,7 +3119,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105790464"/>
+        <c:crossAx val="113474944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2551,7 +3142,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2764,11 +3355,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106237312"/>
-        <c:axId val="106243584"/>
+        <c:axId val="140996608"/>
+        <c:axId val="140998528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106237312"/>
+        <c:axId val="140996608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2792,14 +3383,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106243584"/>
+        <c:crossAx val="140998528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106243584"/>
+        <c:axId val="140998528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2825,7 +3416,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106237312"/>
+        <c:crossAx val="140996608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2848,7 +3439,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3061,11 +3652,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106298368"/>
-        <c:axId val="134419584"/>
+        <c:axId val="141046144"/>
+        <c:axId val="141048064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106298368"/>
+        <c:axId val="141046144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3089,14 +3680,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134419584"/>
+        <c:crossAx val="141048064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134419584"/>
+        <c:axId val="141048064"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3124,7 +3715,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106298368"/>
+        <c:crossAx val="141046144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3147,7 +3738,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3317,11 +3908,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134445696"/>
-        <c:axId val="134456064"/>
+        <c:axId val="141094912"/>
+        <c:axId val="141096832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134445696"/>
+        <c:axId val="141094912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3345,14 +3936,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134456064"/>
+        <c:crossAx val="141096832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134456064"/>
+        <c:axId val="141096832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3380,7 +3971,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134445696"/>
+        <c:crossAx val="141094912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3403,7 +3994,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3573,11 +4164,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134502656"/>
-        <c:axId val="134525312"/>
+        <c:axId val="141118848"/>
+        <c:axId val="141145600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134502656"/>
+        <c:axId val="141118848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3601,14 +4192,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134525312"/>
+        <c:crossAx val="141145600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134525312"/>
+        <c:axId val="141145600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3636,7 +4227,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134502656"/>
+        <c:crossAx val="141118848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3659,7 +4250,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3879,11 +4470,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134544000"/>
-        <c:axId val="134550272"/>
+        <c:axId val="141189120"/>
+        <c:axId val="141191040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134544000"/>
+        <c:axId val="141189120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3907,14 +4498,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134550272"/>
+        <c:crossAx val="141191040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134550272"/>
+        <c:axId val="141191040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3940,7 +4531,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134544000"/>
+        <c:crossAx val="141189120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3963,7 +4554,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4184,11 +4775,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134597632"/>
-        <c:axId val="134608000"/>
+        <c:axId val="141304192"/>
+        <c:axId val="141306112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134597632"/>
+        <c:axId val="141304192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4212,14 +4803,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134608000"/>
+        <c:crossAx val="141306112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134608000"/>
+        <c:axId val="141306112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4245,7 +4836,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134597632"/>
+        <c:crossAx val="141304192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4268,7 +4859,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4310,7 +4901,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4489,11 +5079,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="134638592"/>
-        <c:axId val="134648960"/>
+        <c:axId val="141357440"/>
+        <c:axId val="141359360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134638592"/>
+        <c:axId val="141357440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4514,17 +5104,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134648960"/>
+        <c:crossAx val="141359360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134648960"/>
+        <c:axId val="141359360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4546,18 +5135,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134638592"/>
+        <c:crossAx val="141357440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -4573,7 +5160,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5061,6 +5648,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>326230</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>88107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>90</xdr:col>
+      <xdr:colOff>241631</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>169107</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="31" name="Chart 30"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>369093</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>90</xdr:col>
+      <xdr:colOff>284494</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>116719</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="32" name="Chart 31"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5351,8 +5998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AN95" sqref="AN95"/>
+    <sheetView tabSelected="1" topLeftCell="BM43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BM65" sqref="BM65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>